<commit_message>
Primera prueba haciendo commit y agregando mensaje
</commit_message>
<xml_diff>
--- a/ejemplos_clase/AddSong.xlsx
+++ b/ejemplos_clase/AddSong.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/repo/intro_automation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oelia\Desktop\TERE\intro_automation-master\intro_automation-master\ejemplos_clase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E7D54D9-5FBA-FE4F-AEAD-9F3A6807A37A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8367A3A3-A4EF-471C-A023-D492C1FC8991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{18DC421D-3889-EF4D-B7FC-2C5A42AC8F2F}"/>
+    <workbookView xWindow="2550" yWindow="2550" windowWidth="15375" windowHeight="7995" xr2:uid="{18DC421D-3889-EF4D-B7FC-2C5A42AC8F2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -145,7 +143,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -443,18 +441,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B77FCB89-4431-3C4F-8E60-B607FC6C4202}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="83.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.375" customWidth="1"/>
+    <col min="5" max="5" width="83.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -468,7 +467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="142" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -485,7 +484,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="303" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="303" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>

</xml_diff>